<commit_message>
Revert "Add soccer data"
This reverts commit 2e4f1cf30691a66b96bb5b86337a229e2e5c29fa.
</commit_message>
<xml_diff>
--- a/Soccer social media tracking - 2024.xlsx
+++ b/Soccer social media tracking - 2024.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kvray\OneDrive\Documents\Web Development\NBA TEAMS\nba_socmed_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://spgl-my.sharepoint.com/personal/seth_shafer_spglobal_com/Documents/Documents/OTT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E411BB99-20C4-4995-88FC-31632274987D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{90E8ED9B-057B-4C27-B700-C43A0AF2688E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{89C1FD95-BDB5-4C81-B6B4-8D2B533D4803}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{89C1FD95-BDB5-4C81-B6B4-8D2B533D4803}"/>
   </bookViews>
   <sheets>
     <sheet name="Global" sheetId="1" r:id="rId1"/>
@@ -530,13 +530,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -555,9 +556,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -595,7 +596,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -701,7 +702,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -843,7 +844,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -854,17 +855,17 @@
   <dimension ref="A1:B137"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="D106" sqref="D106"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="11.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.7109375" style="1"/>
+    <col min="1" max="1" width="32.26953125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.90625" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -872,7 +873,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -880,7 +881,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -888,7 +889,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -896,7 +897,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -904,7 +905,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -912,7 +913,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
@@ -920,7 +921,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
@@ -928,7 +929,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
@@ -936,7 +937,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>1</v>
       </c>
@@ -944,7 +945,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
@@ -952,7 +953,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>13</v>
       </c>
@@ -960,7 +961,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>14</v>
       </c>
@@ -968,7 +969,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>15</v>
       </c>
@@ -976,7 +977,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>2</v>
       </c>
@@ -984,7 +985,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>16</v>
       </c>
@@ -992,7 +993,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>17</v>
       </c>
@@ -1000,7 +1001,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>18</v>
       </c>
@@ -1008,7 +1009,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>3</v>
       </c>
@@ -1016,7 +1017,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>19</v>
       </c>
@@ -1024,199 +1025,199 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
         <v>35</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
         <v>37</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
         <v>39</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
         <v>40</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
         <v>41</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
         <v>43</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="s">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
         <v>44</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
         <v>45</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" s="1" t="s">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" s="1" t="s">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>46</v>
       </c>
@@ -1224,7 +1225,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>47</v>
       </c>
@@ -1232,7 +1233,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>48</v>
       </c>
@@ -1240,7 +1241,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>49</v>
       </c>
@@ -1248,7 +1249,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>50</v>
       </c>
@@ -1256,7 +1257,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>51</v>
       </c>
@@ -1264,7 +1265,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>52</v>
       </c>
@@ -1272,7 +1273,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>53</v>
       </c>
@@ -1280,7 +1281,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>54</v>
       </c>
@@ -1288,7 +1289,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>55</v>
       </c>
@@ -1296,7 +1297,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>56</v>
       </c>
@@ -1304,7 +1305,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>57</v>
       </c>
@@ -1312,7 +1313,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>58</v>
       </c>
@@ -1320,7 +1321,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>59</v>
       </c>
@@ -1328,7 +1329,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>60</v>
       </c>
@@ -1336,7 +1337,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>61</v>
       </c>
@@ -1344,7 +1345,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>62</v>
       </c>
@@ -1352,608 +1353,608 @@
         <v>63</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A62" s="3" t="s">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="4" t="s">
         <v>64</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A63" s="3" t="s">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="4" t="s">
         <v>65</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A64" s="3" t="s">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="4" t="s">
         <v>66</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A65" s="3" t="s">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="4" t="s">
         <v>67</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A66" s="3" t="s">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="4" t="s">
         <v>68</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A67" s="3" t="s">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="4" t="s">
         <v>69</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A68" s="3" t="s">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="4" t="s">
         <v>70</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A69" s="3" t="s">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="4" t="s">
         <v>71</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A70" s="3" t="s">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="4" t="s">
         <v>80</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A71" s="3" t="s">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="4" t="s">
         <v>72</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A72" s="3" t="s">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="4" t="s">
         <v>81</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A73" s="3" t="s">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" s="4" t="s">
         <v>73</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A74" s="3" t="s">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="4" t="s">
         <v>74</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A75" s="3" t="s">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="4" t="s">
         <v>75</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A76" s="3" t="s">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" s="4" t="s">
         <v>76</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A77" s="3" t="s">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="4" t="s">
         <v>77</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A78" s="3" t="s">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="4" t="s">
         <v>78</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A79" s="3" t="s">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" s="4" t="s">
         <v>79</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A80" s="3" t="s">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" s="4" t="s">
         <v>83</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A81" s="3" t="s">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" s="4" t="s">
         <v>84</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A82" s="3" t="s">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" s="4" t="s">
         <v>85</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A83" s="3" t="s">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" s="4" t="s">
         <v>86</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A84" s="3" t="s">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="4" t="s">
         <v>87</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A85" s="3" t="s">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" s="4" t="s">
         <v>88</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A86" s="3" t="s">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" s="4" t="s">
         <v>89</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A87" s="3" t="s">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" s="4" t="s">
         <v>90</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A88" s="3" t="s">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" s="4" t="s">
         <v>91</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A89" s="3" t="s">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" s="4" t="s">
         <v>92</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A90" s="3" t="s">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" s="4" t="s">
         <v>93</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A91" s="3" t="s">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" s="4" t="s">
         <v>94</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A92" s="3" t="s">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" s="4" t="s">
         <v>95</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A93" s="3" t="s">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" s="4" t="s">
         <v>96</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A94" s="3" t="s">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" s="4" t="s">
         <v>97</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A95" s="3" t="s">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" s="4" t="s">
         <v>98</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A96" s="3" t="s">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" s="4" t="s">
         <v>99</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A97" s="3" t="s">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" s="4" t="s">
         <v>100</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A98" s="3" t="s">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" s="4" t="s">
         <v>101</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A99" s="3" t="s">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" s="4" t="s">
         <v>102</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A100" s="3" t="s">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" s="4" t="s">
         <v>104</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A101" s="3" t="s">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" s="4" t="s">
         <v>105</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A102" s="3" t="s">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" s="4" t="s">
         <v>106</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A103" s="3" t="s">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" s="4" t="s">
         <v>107</v>
       </c>
       <c r="B103" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A104" s="3" t="s">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" s="4" t="s">
         <v>108</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A105" s="3" t="s">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" s="4" t="s">
         <v>109</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A106" s="3" t="s">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" s="4" t="s">
         <v>110</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A107" s="3" t="s">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" s="4" t="s">
         <v>111</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A108" s="3" t="s">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" s="4" t="s">
         <v>112</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A109" s="3" t="s">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" s="4" t="s">
         <v>113</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A110" s="3" t="s">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" s="4" t="s">
         <v>114</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A111" s="3" t="s">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" s="4" t="s">
         <v>115</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A112" s="3" t="s">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" s="4" t="s">
         <v>116</v>
       </c>
       <c r="B112" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A113" s="3" t="s">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" s="4" t="s">
         <v>117</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A114" s="3" t="s">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" s="4" t="s">
         <v>118</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A115" s="3" t="s">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" s="4" t="s">
         <v>119</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A116" s="3" t="s">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116" s="4" t="s">
         <v>120</v>
       </c>
       <c r="B116" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A117" s="3" t="s">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117" s="4" t="s">
         <v>121</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A118" s="3" t="s">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118" s="4" t="s">
         <v>123</v>
       </c>
       <c r="B118" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A119" s="3" t="s">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119" s="4" t="s">
         <v>124</v>
       </c>
       <c r="B119" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A120" s="3" t="s">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120" s="4" t="s">
         <v>125</v>
       </c>
       <c r="B120" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A121" s="3" t="s">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121" s="4" t="s">
         <v>126</v>
       </c>
       <c r="B121" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A122" s="3" t="s">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122" s="4" t="s">
         <v>127</v>
       </c>
       <c r="B122" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A123" s="3" t="s">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123" s="4" t="s">
         <v>128</v>
       </c>
       <c r="B123" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A124" s="3" t="s">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124" s="4" t="s">
         <v>129</v>
       </c>
       <c r="B124" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A125" s="3" t="s">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125" s="4" t="s">
         <v>130</v>
       </c>
       <c r="B125" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A126" s="3" t="s">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126" s="4" t="s">
         <v>143</v>
       </c>
       <c r="B126" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A127" s="3" t="s">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127" s="4" t="s">
         <v>144</v>
       </c>
       <c r="B127" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A128" s="3" t="s">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128" s="4" t="s">
         <v>133</v>
       </c>
       <c r="B128" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A129" s="3" t="s">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129" s="4" t="s">
         <v>134</v>
       </c>
       <c r="B129" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A130" s="3" t="s">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130" s="4" t="s">
         <v>135</v>
       </c>
       <c r="B130" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A131" s="3" t="s">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131" s="4" t="s">
         <v>136</v>
       </c>
       <c r="B131" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A132" s="3" t="s">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132" s="4" t="s">
         <v>137</v>
       </c>
       <c r="B132" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A133" s="3" t="s">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133" s="4" t="s">
         <v>138</v>
       </c>
       <c r="B133" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A134" s="3" t="s">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134" s="4" t="s">
         <v>139</v>
       </c>
       <c r="B134" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A135" s="3" t="s">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135" s="4" t="s">
         <v>145</v>
       </c>
       <c r="B135" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A136" s="3" t="s">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136" s="4" t="s">
         <v>141</v>
       </c>
       <c r="B136" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A137" s="3" t="s">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137" s="4" t="s">
         <v>142</v>
       </c>
       <c r="B137" s="1" t="s">
@@ -1975,108 +1976,108 @@
       <selection sqref="A1:A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="17" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" s="4" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" s="4" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" s="4" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" s="4" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A10" s="4" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A11" s="4" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A12" s="4" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A13" s="4" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A14" s="4" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A15" s="4" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A16" s="4" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" s="4" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" s="4" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" s="4" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" s="4" t="s">
         <v>142</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Revert "Revert "Add soccer data""
This reverts commit 3fc9e4f3e03d4bb3e88abd311e8006ceac465150.
</commit_message>
<xml_diff>
--- a/Soccer social media tracking - 2024.xlsx
+++ b/Soccer social media tracking - 2024.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://spgl-my.sharepoint.com/personal/seth_shafer_spglobal_com/Documents/Documents/OTT/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kvray\OneDrive\Documents\Web Development\NBA TEAMS\nba_socmed_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{90E8ED9B-057B-4C27-B700-C43A0AF2688E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E411BB99-20C4-4995-88FC-31632274987D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{89C1FD95-BDB5-4C81-B6B4-8D2B533D4803}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{89C1FD95-BDB5-4C81-B6B4-8D2B533D4803}"/>
   </bookViews>
   <sheets>
     <sheet name="Global" sheetId="1" r:id="rId1"/>
@@ -530,14 +530,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -556,9 +555,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -596,7 +595,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -702,7 +701,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -844,7 +843,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -855,17 +854,17 @@
   <dimension ref="A1:B137"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D106" sqref="D106"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="32.26953125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.90625" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="32.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -873,7 +872,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -881,7 +880,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -889,7 +888,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -897,7 +896,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -905,7 +904,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -913,7 +912,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
@@ -921,7 +920,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
@@ -929,7 +928,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
@@ -937,7 +936,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>1</v>
       </c>
@@ -945,7 +944,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
@@ -953,7 +952,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>13</v>
       </c>
@@ -961,7 +960,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>14</v>
       </c>
@@ -969,7 +968,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>15</v>
       </c>
@@ -977,7 +976,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>2</v>
       </c>
@@ -985,7 +984,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>16</v>
       </c>
@@ -993,7 +992,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>17</v>
       </c>
@@ -1001,7 +1000,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>18</v>
       </c>
@@ -1009,7 +1008,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>3</v>
       </c>
@@ -1017,7 +1016,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>19</v>
       </c>
@@ -1025,199 +1024,199 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>46</v>
       </c>
@@ -1225,7 +1224,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>47</v>
       </c>
@@ -1233,7 +1232,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>48</v>
       </c>
@@ -1241,7 +1240,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>49</v>
       </c>
@@ -1249,7 +1248,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>50</v>
       </c>
@@ -1257,7 +1256,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>51</v>
       </c>
@@ -1265,7 +1264,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>52</v>
       </c>
@@ -1273,7 +1272,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>53</v>
       </c>
@@ -1281,7 +1280,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>54</v>
       </c>
@@ -1289,7 +1288,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>55</v>
       </c>
@@ -1297,7 +1296,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>56</v>
       </c>
@@ -1305,7 +1304,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>57</v>
       </c>
@@ -1313,7 +1312,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>58</v>
       </c>
@@ -1321,7 +1320,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>59</v>
       </c>
@@ -1329,7 +1328,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>60</v>
       </c>
@@ -1337,7 +1336,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>61</v>
       </c>
@@ -1345,7 +1344,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>62</v>
       </c>
@@ -1353,608 +1352,608 @@
         <v>63</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="4" t="s">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" s="3" t="s">
         <v>64</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="4" t="s">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63" s="3" t="s">
         <v>65</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="4" t="s">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64" s="3" t="s">
         <v>66</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="4" t="s">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" s="3" t="s">
         <v>67</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="4" t="s">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" s="3" t="s">
         <v>68</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="4" t="s">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" s="3" t="s">
         <v>69</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="4" t="s">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68" s="3" t="s">
         <v>70</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="4" t="s">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" s="3" t="s">
         <v>71</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="4" t="s">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" s="3" t="s">
         <v>80</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="4" t="s">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" s="3" t="s">
         <v>72</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="4" t="s">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72" s="3" t="s">
         <v>81</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="4" t="s">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73" s="3" t="s">
         <v>73</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="4" t="s">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74" s="3" t="s">
         <v>74</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="4" t="s">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75" s="3" t="s">
         <v>75</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="4" t="s">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76" s="3" t="s">
         <v>76</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="4" t="s">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77" s="3" t="s">
         <v>77</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="4" t="s">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78" s="3" t="s">
         <v>78</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="4" t="s">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79" s="3" t="s">
         <v>79</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="4" t="s">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80" s="3" t="s">
         <v>83</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="4" t="s">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" s="3" t="s">
         <v>84</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="4" t="s">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82" s="3" t="s">
         <v>85</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="4" t="s">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83" s="3" t="s">
         <v>86</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="4" t="s">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84" s="3" t="s">
         <v>87</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="4" t="s">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85" s="3" t="s">
         <v>88</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="4" t="s">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86" s="3" t="s">
         <v>89</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="4" t="s">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87" s="3" t="s">
         <v>90</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="4" t="s">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88" s="3" t="s">
         <v>91</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="4" t="s">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A89" s="3" t="s">
         <v>92</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" s="4" t="s">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A90" s="3" t="s">
         <v>93</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" s="4" t="s">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91" s="3" t="s">
         <v>94</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" s="4" t="s">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A92" s="3" t="s">
         <v>95</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="4" t="s">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93" s="3" t="s">
         <v>96</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" s="4" t="s">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A94" s="3" t="s">
         <v>97</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" s="4" t="s">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A95" s="3" t="s">
         <v>98</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" s="4" t="s">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A96" s="3" t="s">
         <v>99</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" s="4" t="s">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A97" s="3" t="s">
         <v>100</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" s="4" t="s">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A98" s="3" t="s">
         <v>101</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" s="4" t="s">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A99" s="3" t="s">
         <v>102</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" s="4" t="s">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A100" s="3" t="s">
         <v>104</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" s="4" t="s">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A101" s="3" t="s">
         <v>105</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A102" s="4" t="s">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A102" s="3" t="s">
         <v>106</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A103" s="4" t="s">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A103" s="3" t="s">
         <v>107</v>
       </c>
       <c r="B103" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A104" s="4" t="s">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A104" s="3" t="s">
         <v>108</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A105" s="4" t="s">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A105" s="3" t="s">
         <v>109</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A106" s="4" t="s">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A106" s="3" t="s">
         <v>110</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107" s="4" t="s">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A107" s="3" t="s">
         <v>111</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A108" s="4" t="s">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A108" s="3" t="s">
         <v>112</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A109" s="4" t="s">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A109" s="3" t="s">
         <v>113</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A110" s="4" t="s">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A110" s="3" t="s">
         <v>114</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A111" s="4" t="s">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A111" s="3" t="s">
         <v>115</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A112" s="4" t="s">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A112" s="3" t="s">
         <v>116</v>
       </c>
       <c r="B112" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A113" s="4" t="s">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A113" s="3" t="s">
         <v>117</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A114" s="4" t="s">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A114" s="3" t="s">
         <v>118</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A115" s="4" t="s">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A115" s="3" t="s">
         <v>119</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A116" s="4" t="s">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A116" s="3" t="s">
         <v>120</v>
       </c>
       <c r="B116" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A117" s="4" t="s">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A117" s="3" t="s">
         <v>121</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A118" s="4" t="s">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A118" s="3" t="s">
         <v>123</v>
       </c>
       <c r="B118" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A119" s="4" t="s">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A119" s="3" t="s">
         <v>124</v>
       </c>
       <c r="B119" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A120" s="4" t="s">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A120" s="3" t="s">
         <v>125</v>
       </c>
       <c r="B120" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A121" s="4" t="s">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A121" s="3" t="s">
         <v>126</v>
       </c>
       <c r="B121" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A122" s="4" t="s">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A122" s="3" t="s">
         <v>127</v>
       </c>
       <c r="B122" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A123" s="4" t="s">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A123" s="3" t="s">
         <v>128</v>
       </c>
       <c r="B123" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A124" s="4" t="s">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A124" s="3" t="s">
         <v>129</v>
       </c>
       <c r="B124" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A125" s="4" t="s">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A125" s="3" t="s">
         <v>130</v>
       </c>
       <c r="B125" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A126" s="4" t="s">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A126" s="3" t="s">
         <v>143</v>
       </c>
       <c r="B126" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A127" s="4" t="s">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A127" s="3" t="s">
         <v>144</v>
       </c>
       <c r="B127" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A128" s="4" t="s">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A128" s="3" t="s">
         <v>133</v>
       </c>
       <c r="B128" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A129" s="4" t="s">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A129" s="3" t="s">
         <v>134</v>
       </c>
       <c r="B129" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A130" s="4" t="s">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A130" s="3" t="s">
         <v>135</v>
       </c>
       <c r="B130" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A131" s="4" t="s">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A131" s="3" t="s">
         <v>136</v>
       </c>
       <c r="B131" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A132" s="4" t="s">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A132" s="3" t="s">
         <v>137</v>
       </c>
       <c r="B132" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A133" s="4" t="s">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A133" s="3" t="s">
         <v>138</v>
       </c>
       <c r="B133" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A134" s="4" t="s">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A134" s="3" t="s">
         <v>139</v>
       </c>
       <c r="B134" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A135" s="4" t="s">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A135" s="3" t="s">
         <v>145</v>
       </c>
       <c r="B135" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A136" s="4" t="s">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A136" s="3" t="s">
         <v>141</v>
       </c>
       <c r="B136" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A137" s="4" t="s">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A137" s="3" t="s">
         <v>142</v>
       </c>
       <c r="B137" s="1" t="s">
@@ -1976,108 +1975,108 @@
       <selection sqref="A1:A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A8" s="4" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A9" s="4" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A10" s="4" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A11" s="4" t="s">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A12" s="4" t="s">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A13" s="4" t="s">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A14" s="4" t="s">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A15" s="4" t="s">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A16" s="4" t="s">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A17" s="4" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A18" s="4" t="s">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A19" s="4" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A20" s="4" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
         <v>142</v>
       </c>
     </row>

</xml_diff>